<commit_message>
i updated xl sheet
</commit_message>
<xml_diff>
--- a/pv_template.xlsx
+++ b/pv_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krazy\Box\UCLA\Research\ITV-PV\Marvin PV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhivinod/Desktop/sacklabintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5521C9BA-45BD-47AE-BE5A-9DE07CE958CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C77E24D-B1BC-D141-AABC-9A8AC191684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19308" yWindow="-108" windowWidth="19416" windowHeight="15576" tabRatio="738" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" tabRatio="738" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="19" r:id="rId1"/>
@@ -8145,31 +8145,31 @@
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="109" t="s">
         <v>90</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="59">
         <v>1</v>
       </c>
@@ -8264,7 +8264,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="59">
         <v>2</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="59">
         <v>3</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="59">
         <v>4</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="59">
         <v>5</v>
       </c>
@@ -8456,7 +8456,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="59">
         <v>6</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="109" t="s">
         <v>83</v>
       </c>
@@ -8565,7 +8565,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="109" t="s">
         <v>84</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="59"/>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
@@ -8645,7 +8645,7 @@
       <c r="N10" s="59"/>
       <c r="O10" s="59"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="109"/>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
@@ -8662,7 +8662,7 @@
       <c r="N11" s="59"/>
       <c r="O11" s="59"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="59"/>
       <c r="B12" s="59"/>
       <c r="C12" s="59"/>
@@ -8679,6 +8679,11 @@
       <c r="N12" s="59"/>
       <c r="O12" s="59"/>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8693,33 +8698,33 @@
       <selection activeCell="C10" activeCellId="1" sqref="A10:A19 C10:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.21875" customWidth="1"/>
-    <col min="13" max="13" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -8729,7 +8734,7 @@
       <c r="E2" s="55"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
@@ -8740,7 +8745,7 @@
       </c>
       <c r="E3" s="55"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
         <v>3</v>
       </c>
@@ -8749,7 +8754,7 @@
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
@@ -8763,7 +8768,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="52" t="s">
         <v>87</v>
       </c>
@@ -8774,14 +8779,14 @@
       <c r="M6" s="7"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="D7" s="2"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="115" t="s">
         <v>5</v>
       </c>
@@ -8828,7 +8833,7 @@
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41"/>
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
@@ -8851,43 +8856,43 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="42"/>
       <c r="B10" s="43" t="e">
-        <f t="shared" ref="B10:B20" si="0">-1/A10</f>
+        <f t="shared" ref="B10:B19" si="0">-1/A10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C10" s="44"/>
       <c r="D10" s="45">
-        <f t="shared" ref="D10:D20" si="1">C10-$B$3-$B$4-$B$5</f>
+        <f t="shared" ref="D10:D19" si="1">C10-$B$3-$B$4-$B$5</f>
         <v>0</v>
       </c>
       <c r="E10" s="46" t="e">
-        <f t="shared" ref="E10:E20" si="2">(D10/$B$24)</f>
+        <f t="shared" ref="E10:E19" si="2">(D10/$B$24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F10" s="67" t="e">
-        <f t="shared" ref="F10:F20" si="3">100*E10</f>
+        <f t="shared" ref="F10:F19" si="3">100*E10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G10" s="46" t="e">
-        <f t="shared" ref="G10:G20" si="4">100-F10</f>
+        <f t="shared" ref="G10:G19" si="4">100-F10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H10" s="46" t="e">
-        <f t="shared" ref="H10:H20" si="5">(E10-N$11/100)/(1-N$11/100)</f>
+        <f t="shared" ref="H10:H18" si="5">(E10-N$11/100)/(1-N$11/100)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I10" s="67" t="e">
-        <f t="shared" ref="I10:I20" si="6">H10*100</f>
+        <f t="shared" ref="I10:I18" si="6">H10*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J10" s="47" t="e">
-        <f t="shared" ref="J10:J20" si="7">-1/($K$24+$K$23*G10)</f>
+        <f t="shared" ref="J10:J19" si="7">-1/($K$24+$K$23*G10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="47" t="e">
-        <f t="shared" ref="K10:K20" si="8">A10-J10</f>
+        <f t="shared" ref="K10:K19" si="8">A10-J10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="86" t="s">
@@ -8901,7 +8906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="e">
         <f t="shared" si="0"/>
@@ -8951,7 +8956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="48"/>
       <c r="B12" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9001,7 +9006,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9051,7 +9056,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9101,7 +9106,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="48"/>
       <c r="B15" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9151,7 +9156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="48"/>
       <c r="B16" s="71" t="e">
         <f t="shared" si="0"/>
@@ -9201,7 +9206,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="48"/>
       <c r="B17" s="71" t="e">
         <f t="shared" si="0"/>
@@ -9251,7 +9256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
       <c r="B18" s="71" t="e">
         <f t="shared" si="0"/>
@@ -9301,7 +9306,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
       <c r="B19" s="71" t="e">
         <f t="shared" si="0"/>
@@ -9351,7 +9356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="64"/>
       <c r="B20" s="71"/>
       <c r="C20" s="72"/>
@@ -9371,7 +9376,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77"/>
       <c r="B21" s="52"/>
       <c r="C21" s="78"/>
@@ -9391,7 +9396,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>40</v>
       </c>
@@ -9406,7 +9411,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -9432,7 +9437,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -9456,7 +9461,7 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J25" s="61" t="s">
         <v>43</v>
       </c>
@@ -9467,33 +9472,33 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="O31" s="6"/>
     </row>
-    <row r="35" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="14:15" x14ac:dyDescent="0.2">
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="14:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="14:15" x14ac:dyDescent="0.2">
       <c r="O36" s="2"/>
     </row>
   </sheetData>
@@ -9512,32 +9517,32 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -9547,7 +9552,7 @@
       <c r="E2" s="55"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
@@ -9558,7 +9563,7 @@
       </c>
       <c r="E3" s="56"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
         <v>3</v>
       </c>
@@ -9571,7 +9576,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
@@ -9585,14 +9590,14 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="115" t="s">
         <v>5</v>
       </c>
@@ -9639,7 +9644,7 @@
       <c r="P7" s="32"/>
       <c r="Q7" s="32"/>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
@@ -9662,7 +9667,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="48"/>
       <c r="B9" s="43" t="e">
         <f>-1/A9</f>
@@ -9712,7 +9717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="43" t="e">
         <f t="shared" ref="B10:B19" si="0">-1/A10</f>
@@ -9763,7 +9768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9814,7 +9819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9865,7 +9870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9916,7 +9921,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="42"/>
       <c r="B14" s="43" t="e">
         <f t="shared" si="0"/>
@@ -9966,7 +9971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
       <c r="B15" s="50" t="e">
         <f t="shared" si="0"/>
@@ -10016,7 +10021,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="116"/>
       <c r="B16" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10066,7 +10071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="42"/>
       <c r="B17" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10116,7 +10121,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="42"/>
       <c r="B18" s="71" t="e">
         <f t="shared" si="0"/>
@@ -10166,7 +10171,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="42"/>
       <c r="B19" s="71" t="e">
         <f t="shared" si="0"/>
@@ -10214,7 +10219,7 @@
       </c>
       <c r="O19" s="59"/>
     </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="113"/>
       <c r="B20" s="52"/>
       <c r="C20" s="79"/>
@@ -10235,17 +10240,17 @@
       </c>
       <c r="O20" s="59"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="M21" s="80"/>
       <c r="N21" s="81"/>
       <c r="O21" s="59"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P22" s="5"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>40</v>
       </c>
@@ -10260,7 +10265,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -10286,7 +10291,7 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -10311,7 +10316,7 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J26" s="1" t="s">
         <v>43</v>
       </c>
@@ -10322,62 +10327,62 @@
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P27" t="s">
         <v>85</v>
       </c>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="35"/>
       <c r="B44" s="36"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="37"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="37"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="38"/>
       <c r="B48" s="37"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
       <c r="B49" s="12"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
       <c r="B51" s="36"/>
     </row>
@@ -10397,32 +10402,32 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -10433,7 +10438,7 @@
       <c r="F2" s="70"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
@@ -10444,7 +10449,7 @@
       </c>
       <c r="E3" s="56"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
         <v>86</v>
       </c>
@@ -10453,7 +10458,7 @@
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
@@ -10467,14 +10472,14 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
@@ -10521,7 +10526,7 @@
       <c r="P7" s="32"/>
       <c r="Q7" s="32"/>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M8" s="84" t="s">
         <v>18</v>
       </c>
@@ -10533,7 +10538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="48"/>
       <c r="B9" s="43" t="e">
         <f t="shared" ref="B9:B18" si="0">-1/A9</f>
@@ -10545,31 +10550,31 @@
         <v>0</v>
       </c>
       <c r="E9" s="49" t="e">
-        <f>(D9/$B$22)</f>
+        <f t="shared" ref="E9:E18" si="1">(D9/$B$22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F9" s="46" t="e">
-        <f t="shared" ref="F9" si="1">100*E9</f>
+        <f t="shared" ref="F9" si="2">100*E9</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G9" s="46" t="e">
-        <f t="shared" ref="G9" si="2">100-F9</f>
+        <f t="shared" ref="G9" si="3">100-F9</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H9" s="41" t="e">
-        <f t="shared" ref="H9" si="3">(E9-N$10/100)/(1-N$10/100)</f>
+        <f t="shared" ref="H9" si="4">(E9-N$10/100)/(1-N$10/100)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I9" s="41" t="e">
-        <f t="shared" ref="I9" si="4">H9*100</f>
+        <f t="shared" ref="I9" si="5">H9*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J9" s="47" t="e">
-        <f>-1/($K$22+$K$21*G9)</f>
+        <f t="shared" ref="J9:J18" si="6">-1/($K$22+$K$21*G9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K9" s="47" t="e">
-        <f t="shared" ref="K9" si="5">A9-J9</f>
+        <f t="shared" ref="K9" si="7">A9-J9</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="86" t="s">
@@ -10583,7 +10588,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10591,35 +10596,35 @@
       </c>
       <c r="C10" s="66"/>
       <c r="D10" s="45">
-        <f t="shared" ref="D10:D18" si="6">C10-$B$3-$B$4-$B$5</f>
+        <f t="shared" ref="D10:D18" si="8">C10-$B$3-$B$4-$B$5</f>
         <v>0</v>
       </c>
       <c r="E10" s="49" t="e">
-        <f>(D10/$B$22)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F10" s="46" t="e">
-        <f t="shared" ref="F10:F17" si="7">100*E10</f>
+        <f t="shared" ref="F10:F17" si="9">100*E10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G10" s="46" t="e">
-        <f t="shared" ref="G10:G17" si="8">100-F10</f>
+        <f t="shared" ref="G10:G17" si="10">100-F10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H10" s="41" t="e">
-        <f t="shared" ref="H10:H18" si="9">(E10-N$10/100)/(1-N$10/100)</f>
+        <f t="shared" ref="H10:H18" si="11">(E10-N$10/100)/(1-N$10/100)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I10" s="41" t="e">
-        <f t="shared" ref="I10:I18" si="10">H10*100</f>
+        <f t="shared" ref="I10:I18" si="12">H10*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J10" s="47" t="e">
-        <f>-1/($K$22+$K$21*G10)</f>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="47" t="e">
-        <f t="shared" ref="K10:K18" si="11">A10-J10</f>
+        <f t="shared" ref="K10:K18" si="13">A10-J10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="92" t="s">
@@ -10633,7 +10638,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10641,35 +10646,35 @@
       </c>
       <c r="C11" s="44"/>
       <c r="D11" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="41" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="41" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="47" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="49" t="e">
-        <f>(D11/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="46" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I11" s="41" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="47" t="e">
-        <f>-1/($K$22+$K$21*G11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="47" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="89" t="s">
@@ -10683,7 +10688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10691,35 +10696,35 @@
       </c>
       <c r="C12" s="44"/>
       <c r="D12" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="41" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I12" s="41" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="47" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="49" t="e">
-        <f>(D12/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" s="46" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I12" s="41" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="47" t="e">
-        <f>-1/($K$22+$K$21*G12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K12" s="47" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="86" t="s">
@@ -10733,7 +10738,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10741,35 +10746,35 @@
       </c>
       <c r="C13" s="66"/>
       <c r="D13" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="41" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13" s="41" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="47" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="49" t="e">
-        <f>(D13/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="46" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G13" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" s="41" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="47" t="e">
-        <f>-1/($K$22+$K$21*G13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K13" s="47" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="89" t="s">
@@ -10783,7 +10788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10791,35 +10796,35 @@
       </c>
       <c r="C14" s="44"/>
       <c r="D14" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="41" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14" s="41" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="47" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="49" t="e">
-        <f>(D14/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="46" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G14" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I14" s="41" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" s="47" t="e">
-        <f>-1/($K$22+$K$21*G14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K14" s="47" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="86" t="s">
@@ -10833,7 +10838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
       <c r="B15" s="43" t="e">
         <f t="shared" si="0"/>
@@ -10841,35 +10846,35 @@
       </c>
       <c r="C15" s="66"/>
       <c r="D15" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G15" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="41" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="41" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="47" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="49" t="e">
-        <f>(D15/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="46" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="41" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="41" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="47" t="e">
-        <f>-1/($K$22+$K$21*G15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K15" s="47" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="86" t="s">
@@ -10883,7 +10888,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
       <c r="B16" s="50" t="e">
         <f t="shared" si="0"/>
@@ -10891,35 +10896,35 @@
       </c>
       <c r="C16" s="44"/>
       <c r="D16" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="46" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G16" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="65" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="65" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="47" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="49" t="e">
-        <f>(D16/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F16" s="46" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G16" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16" s="65" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="65" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="47" t="e">
-        <f>-1/($K$22+$K$21*G16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="47" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="86" t="s">
@@ -10933,7 +10938,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="42"/>
       <c r="B17" s="71" t="e">
         <f t="shared" si="0"/>
@@ -10941,35 +10946,35 @@
       </c>
       <c r="C17" s="66"/>
       <c r="D17" s="45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="74" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="75" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="46" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="65" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="65" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="64" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="74" t="e">
-        <f>(D17/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F17" s="75" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G17" s="46" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="65" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I17" s="65" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="64" t="e">
-        <f>-1/($K$22+$K$21*G17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="64" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="86" t="s">
@@ -10983,7 +10988,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="42"/>
       <c r="B18" s="71" t="e">
         <f t="shared" si="0"/>
@@ -10991,35 +10996,35 @@
       </c>
       <c r="C18" s="66"/>
       <c r="D18" s="73">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="74" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="75" t="e">
+        <f t="shared" ref="F18" si="14">100*E18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="46" t="e">
+        <f t="shared" ref="G18" si="15">100-F18</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="65" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="65" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="64" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="74" t="e">
-        <f>(D18/$B$22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="75" t="e">
-        <f t="shared" ref="F18" si="12">100*E18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="46" t="e">
-        <f t="shared" ref="G18" si="13">100-F18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="65" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="65" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="64" t="e">
-        <f>-1/($K$22+$K$21*G18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="64" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="86" t="s">
@@ -11033,7 +11038,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>85</v>
       </c>
@@ -11046,7 +11051,7 @@
       </c>
       <c r="O19" s="59"/>
     </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
@@ -11068,7 +11073,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -11094,7 +11099,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -11119,7 +11124,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J23" s="1" t="s">
         <v>43</v>
       </c>
@@ -11134,66 +11139,66 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P25" t="s">
         <v>85</v>
       </c>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="36"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="37"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="37"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
     </row>
-    <row r="45" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="38"/>
       <c r="B45" s="37"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="36"/>
     </row>
@@ -11213,32 +11218,32 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:243" x14ac:dyDescent="0.2">
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -11248,7 +11253,7 @@
       <c r="E2" s="55"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
@@ -11259,7 +11264,7 @@
       </c>
       <c r="E3" s="56"/>
     </row>
-    <row r="4" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
         <v>86</v>
       </c>
@@ -11268,7 +11273,7 @@
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
-    <row r="5" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
@@ -11282,14 +11287,14 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:243" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:243" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:243" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:243" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
@@ -11562,7 +11567,7 @@
       <c r="IH7" s="41"/>
       <c r="II7" s="41"/>
     </row>
-    <row r="8" spans="1:243" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:243" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M8" s="84" t="s">
         <v>18</v>
       </c>
@@ -11802,7 +11807,7 @@
       <c r="IH8" s="41"/>
       <c r="II8" s="41"/>
     </row>
-    <row r="9" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A9" s="48"/>
       <c r="B9" s="43" t="e">
         <f t="shared" ref="B9:B19" si="0">-1/A9</f>
@@ -12081,7 +12086,7 @@
       <c r="IH9" s="41"/>
       <c r="II9" s="41"/>
     </row>
-    <row r="10" spans="1:243" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:243" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="43" t="e">
         <f t="shared" si="0"/>
@@ -12360,7 +12365,7 @@
       <c r="IH10" s="41"/>
       <c r="II10" s="41"/>
     </row>
-    <row r="11" spans="1:243" s="34" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:243" s="34" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="e">
         <f t="shared" si="0"/>
@@ -12639,7 +12644,7 @@
       <c r="IH11" s="41"/>
       <c r="II11" s="41"/>
     </row>
-    <row r="12" spans="1:243" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:243" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="e">
         <f t="shared" si="0"/>
@@ -12918,7 +12923,7 @@
       <c r="IH12" s="41"/>
       <c r="II12" s="41"/>
     </row>
-    <row r="13" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="43" t="e">
         <f t="shared" si="0"/>
@@ -13197,7 +13202,7 @@
       <c r="IH13" s="41"/>
       <c r="II13" s="41"/>
     </row>
-    <row r="14" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="43" t="e">
         <f t="shared" si="0"/>
@@ -13476,7 +13481,7 @@
       <c r="IH14" s="41"/>
       <c r="II14" s="41"/>
     </row>
-    <row r="15" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
       <c r="B15" s="43" t="e">
         <f t="shared" si="0"/>
@@ -13755,7 +13760,7 @@
       <c r="IH15" s="41"/>
       <c r="II15" s="41"/>
     </row>
-    <row r="16" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
       <c r="B16" s="50" t="e">
         <f t="shared" si="0"/>
@@ -14034,7 +14039,7 @@
       <c r="IH16" s="41"/>
       <c r="II16" s="41"/>
     </row>
-    <row r="17" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A17" s="48"/>
       <c r="B17" s="71" t="e">
         <f t="shared" si="0"/>
@@ -14312,7 +14317,7 @@
       <c r="IH17" s="41"/>
       <c r="II17" s="41"/>
     </row>
-    <row r="18" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A18" s="48"/>
       <c r="B18" s="71" t="e">
         <f t="shared" si="0"/>
@@ -14590,7 +14595,7 @@
       <c r="IH18" s="41"/>
       <c r="II18" s="41"/>
     </row>
-    <row r="19" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A19" s="48"/>
       <c r="B19" s="71" t="e">
         <f t="shared" si="0"/>
@@ -14866,7 +14871,7 @@
       <c r="IH19" s="41"/>
       <c r="II19" s="41"/>
     </row>
-    <row r="20" spans="1:243" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:243" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
@@ -15114,7 +15119,7 @@
       <c r="IH20" s="41"/>
       <c r="II20" s="41"/>
     </row>
-    <row r="21" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:243" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -15366,7 +15371,7 @@
       <c r="IH21" s="41"/>
       <c r="II21" s="41"/>
     </row>
-    <row r="22" spans="1:243" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:243" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -15388,7 +15393,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:243" x14ac:dyDescent="0.2">
       <c r="J23" s="1" t="s">
         <v>43</v>
       </c>
@@ -15403,66 +15408,66 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:243" x14ac:dyDescent="0.2">
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:243" x14ac:dyDescent="0.2">
       <c r="P25" t="s">
         <v>85</v>
       </c>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:243" x14ac:dyDescent="0.2">
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:243" x14ac:dyDescent="0.2">
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:243" x14ac:dyDescent="0.2">
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:243" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:243" x14ac:dyDescent="0.2">
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="36"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="37"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="37"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
     </row>
-    <row r="45" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="38"/>
       <c r="B45" s="37"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="36"/>
     </row>
@@ -15482,32 +15487,32 @@
       <selection activeCell="A10" sqref="A10:K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.2">
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -15517,7 +15522,7 @@
       <c r="E2" s="55"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
@@ -15528,7 +15533,7 @@
       </c>
       <c r="E3" s="56"/>
     </row>
-    <row r="4" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
         <v>86</v>
       </c>
@@ -15537,7 +15542,7 @@
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
-    <row r="5" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
@@ -15551,14 +15556,14 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:112" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:112" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:112" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:112" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
@@ -15605,7 +15610,7 @@
       <c r="P7" s="32"/>
       <c r="Q7" s="32"/>
     </row>
-    <row r="8" spans="1:112" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:112" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M8" s="84" t="s">
         <v>18</v>
       </c>
@@ -15617,7 +15622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.2">
       <c r="L9" s="41"/>
       <c r="M9" s="86" t="s">
         <v>20</v>
@@ -15630,7 +15635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:112" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:112" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="43" t="e">
         <f t="shared" ref="B10:B20" si="0">-1/A10</f>
@@ -15681,7 +15686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:112" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:112" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="e">
         <f t="shared" si="0"/>
@@ -15829,7 +15834,7 @@
       <c r="DG11" s="41"/>
       <c r="DH11" s="41"/>
     </row>
-    <row r="12" spans="1:112" s="34" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:112" s="34" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="e">
         <f t="shared" si="0"/>
@@ -15977,7 +15982,7 @@
       <c r="DG12" s="41"/>
       <c r="DH12" s="41"/>
     </row>
-    <row r="13" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="43" t="e">
         <f t="shared" si="0"/>
@@ -16125,7 +16130,7 @@
       <c r="DG13" s="41"/>
       <c r="DH13" s="41"/>
     </row>
-    <row r="14" spans="1:112" s="34" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:112" s="34" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
       <c r="B14" s="43" t="e">
         <f t="shared" si="0"/>
@@ -16273,7 +16278,7 @@
       <c r="DG14" s="41"/>
       <c r="DH14" s="41"/>
     </row>
-    <row r="15" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
       <c r="B15" s="43" t="e">
         <f t="shared" si="0"/>
@@ -16421,7 +16426,7 @@
       <c r="DG15" s="41"/>
       <c r="DH15" s="41"/>
     </row>
-    <row r="16" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
       <c r="B16" s="50" t="e">
         <f t="shared" si="0"/>
@@ -16569,7 +16574,7 @@
       <c r="DG16" s="41"/>
       <c r="DH16" s="41"/>
     </row>
-    <row r="17" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A17" s="42"/>
       <c r="B17" s="43" t="e">
         <f t="shared" si="0"/>
@@ -16717,7 +16722,7 @@
       <c r="DG17" s="41"/>
       <c r="DH17" s="41"/>
     </row>
-    <row r="18" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A18" s="42"/>
       <c r="B18" s="71" t="e">
         <f t="shared" si="0"/>
@@ -16864,7 +16869,7 @@
       <c r="DG18" s="41"/>
       <c r="DH18" s="41"/>
     </row>
-    <row r="19" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A19" s="42"/>
       <c r="B19" s="71" t="e">
         <f t="shared" si="0"/>
@@ -17009,7 +17014,7 @@
       <c r="DG19" s="41"/>
       <c r="DH19" s="41"/>
     </row>
-    <row r="20" spans="1:112" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:112" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42"/>
       <c r="B20" s="71" t="e">
         <f t="shared" si="0"/>
@@ -17059,7 +17064,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
@@ -17074,7 +17079,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:112" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -17101,7 +17106,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:112" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:112" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -17127,7 +17132,7 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:112" x14ac:dyDescent="0.2">
       <c r="G24" s="46"/>
       <c r="J24" s="1" t="s">
         <v>43</v>
@@ -17139,7 +17144,7 @@
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:112" x14ac:dyDescent="0.2">
       <c r="M25" t="s">
         <v>89</v>
       </c>
@@ -17149,55 +17154,55 @@
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:112" x14ac:dyDescent="0.2">
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.2">
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:112" x14ac:dyDescent="0.2">
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:112" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:112" x14ac:dyDescent="0.2">
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="35"/>
       <c r="B42" s="36"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="37"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="37"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="38"/>
       <c r="B46" s="37"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
       <c r="B49" s="36"/>
     </row>
@@ -17217,32 +17222,32 @@
       <selection activeCell="A9" sqref="A9:K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5546875" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.5" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -17252,7 +17257,7 @@
       <c r="E2" s="55"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
@@ -17263,14 +17268,14 @@
       </c>
       <c r="E3" s="117"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="55"/>
       <c r="B4" s="69"/>
       <c r="C4" s="55"/>
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
@@ -17284,14 +17289,14 @@
       <c r="M5" s="7"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>5</v>
       </c>
@@ -17338,7 +17343,7 @@
       <c r="P7" s="32"/>
       <c r="Q7" s="32"/>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="M8" s="84" t="s">
         <v>18</v>
       </c>
@@ -17350,7 +17355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="48"/>
       <c r="B9" s="43" t="e">
         <f t="shared" ref="B9:B19" si="0">-1/A9</f>
@@ -17400,7 +17405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17450,7 +17455,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17500,7 +17505,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="42"/>
       <c r="B12" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17550,7 +17555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="48"/>
       <c r="B13" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17600,7 +17605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="48"/>
       <c r="B14" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17650,7 +17655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="42"/>
       <c r="B15" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17700,7 +17705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
       <c r="B16" s="50" t="e">
         <f t="shared" si="0"/>
@@ -17750,7 +17755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="42"/>
       <c r="B17" s="43" t="e">
         <f t="shared" si="0"/>
@@ -17800,7 +17805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
       <c r="B18" s="71" t="e">
         <f t="shared" si="0"/>
@@ -17850,7 +17855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="42"/>
       <c r="B19" s="71" t="e">
         <f t="shared" si="0"/>
@@ -17898,7 +17903,7 @@
       </c>
       <c r="O19" s="59"/>
     </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>40</v>
       </c>
@@ -17920,7 +17925,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -17946,7 +17951,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -17968,7 +17973,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="J23" s="1" t="s">
         <v>43</v>
       </c>
@@ -17983,66 +17988,66 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P25" t="s">
         <v>85</v>
       </c>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="35"/>
       <c r="B41" s="36"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="37"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="37"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
     </row>
-    <row r="45" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="38"/>
       <c r="B45" s="37"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="36"/>
     </row>
@@ -18065,12 +18070,12 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>46</v>
       </c>
@@ -18079,7 +18084,7 @@
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>47</v>
       </c>
@@ -18088,7 +18093,7 @@
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>48</v>
       </c>
@@ -18097,7 +18102,7 @@
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
     </row>
-    <row r="5" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
         <v>49</v>
       </c>
@@ -18120,7 +18125,7 @@
       <c r="R5" s="39"/>
       <c r="S5" s="39"/>
     </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -18128,7 +18133,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -18152,7 +18157,7 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -18171,7 +18176,7 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
     </row>
-    <row r="9" spans="1:19" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="s">
         <v>54</v>
       </c>
@@ -18194,7 +18199,7 @@
       <c r="R9" s="27"/>
       <c r="S9" s="39"/>
     </row>
-    <row r="10" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -18218,7 +18223,7 @@
       <c r="Q10" s="15"/>
       <c r="R10" s="15"/>
     </row>
-    <row r="11" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -18242,7 +18247,7 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -18267,7 +18272,7 @@
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
     </row>
-    <row r="13" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -18292,7 +18297,7 @@
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
     </row>
-    <row r="14" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -18316,7 +18321,7 @@
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
     </row>
-    <row r="15" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -18335,7 +18340,7 @@
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
     </row>
-    <row r="16" spans="1:19" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="s">
         <v>63</v>
       </c>
@@ -18358,7 +18363,7 @@
       <c r="R16" s="27"/>
       <c r="S16" s="39"/>
     </row>
-    <row r="17" spans="1:18" ht="18" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -18382,7 +18387,7 @@
       <c r="Q17" s="15"/>
       <c r="R17" s="15"/>
     </row>
-    <row r="18" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -18406,7 +18411,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
     </row>
-    <row r="19" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -18430,7 +18435,7 @@
       <c r="Q19" s="15"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -18454,7 +18459,7 @@
       <c r="Q20" s="15"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -18478,7 +18483,7 @@
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -18502,7 +18507,7 @@
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -18526,7 +18531,7 @@
       <c r="Q23" s="15"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -18550,7 +18555,7 @@
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -18574,7 +18579,7 @@
       <c r="Q25" s="15"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
@@ -18592,7 +18597,7 @@
       <c r="Q26" s="15"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:18" s="26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
         <v>77</v>
       </c>
@@ -18614,7 +18619,7 @@
       <c r="Q27" s="27"/>
       <c r="R27" s="27"/>
     </row>
-    <row r="28" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -18638,7 +18643,7 @@
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
     </row>
-    <row r="29" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -18662,7 +18667,7 @@
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -18686,7 +18691,7 @@
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -18710,7 +18715,7 @@
       <c r="Q31" s="15"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -18734,7 +18739,7 @@
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>

</xml_diff>